<commit_message>
Edit A* to -1 from f(n). Added LGS version which still performed same as Graph search with update on Astar. Double check definition of LGS.
</commit_message>
<xml_diff>
--- a/Project 1/Tmp.xlsx
+++ b/Project 1/Tmp.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Drew\Desktop\CS3243\Project 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pryo\Desktop\CS3243 GH\Project 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8DF8D36-5DA6-42F9-86D4-A4FFA16C6DEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7842796-69D7-410C-913B-C130C31E09ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4920" yWindow="0" windowWidth="21600" windowHeight="13425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -396,10 +396,13 @@
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="20" max="20" width="58.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1">

</xml_diff>